<commit_message>
tracking changes in nbs
</commit_message>
<xml_diff>
--- a/louisiana/transformations/templates/calibrated/louisiana/model_input_variables_louisiana_se_calibrated.xlsx
+++ b/louisiana/transformations/templates/calibrated/louisiana/model_input_variables_louisiana_se_calibrated.xlsx
@@ -8,14 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
-    <sheet name="strategy_id-6002" sheetId="2" r:id="rId2"/>
+    <sheet name="strategy_id-6004" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
   <si>
     <t>subsector</t>
   </si>
@@ -42,6 +42,114 @@
   </si>
   <si>
     <t>min_35</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
   </si>
   <si>
     <t>Economy</t>
@@ -472,127 +580,130 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>7</v>
-      </c>
-      <c r="R1" s="1">
-        <v>8</v>
-      </c>
-      <c r="S1" s="1">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="1">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="1">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="1">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="W1" s="1">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="1">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" s="1">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="1">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AD1" s="1">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AE1" s="1">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AF1" s="1">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AG1" s="1">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AH1" s="1">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AI1" s="1">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AJ1" s="1">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AK1" s="1">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AL1" s="1">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AM1" s="1">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AN1" s="1">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AO1" s="1">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AP1" s="1">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AQ1" s="1">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="1">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AS1" s="1">
+      <c r="AJ1" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:45">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>47</v>
+      </c>
+      <c r="C2">
+        <v>52</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="J2">
         <v>232.458</v>
@@ -705,10 +816,10 @@
     </row>
     <row r="3" spans="1:45">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -827,16 +938,16 @@
     </row>
     <row r="4" spans="1:45">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -949,10 +1060,10 @@
     </row>
     <row r="5" spans="1:45">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1071,13 +1182,13 @@
     </row>
     <row r="6" spans="1:45">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="C6">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -1196,10 +1307,10 @@
     </row>
     <row r="7" spans="1:45">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -1318,10 +1429,10 @@
     </row>
     <row r="8" spans="1:45">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1440,10 +1551,10 @@
     </row>
     <row r="9" spans="1:45">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -1562,10 +1673,10 @@
     </row>
     <row r="10" spans="1:45">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -1684,16 +1795,19 @@
     </row>
     <row r="11" spans="1:45">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>56</v>
+      </c>
+      <c r="C11">
+        <v>53</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>1.075</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>0.925</v>
       </c>
       <c r="J11">
         <v>1270673.58425</v>
@@ -1806,16 +1920,19 @@
     </row>
     <row r="12" spans="1:45">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>57</v>
+      </c>
+      <c r="C12">
+        <v>53</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>1.075</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>0.925</v>
       </c>
       <c r="J12">
         <v>3324890.91575</v>
@@ -1967,124 +2084,124 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>7</v>
-      </c>
-      <c r="R1" s="1">
-        <v>8</v>
-      </c>
-      <c r="S1" s="1">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="1">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="1">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="1">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="W1" s="1">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="1">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" s="1">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="1">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AD1" s="1">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AE1" s="1">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AF1" s="1">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AG1" s="1">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AH1" s="1">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AI1" s="1">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AJ1" s="1">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AK1" s="1">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AL1" s="1">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AM1" s="1">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AN1" s="1">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AO1" s="1">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AP1" s="1">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AQ1" s="1">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="1">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AS1" s="1">
+      <c r="AJ1" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:45">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="C2">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H2">
         <v>1</v>

</xml_diff>

<commit_message>
updated louisiana inputs and data
</commit_message>
<xml_diff>
--- a/louisiana/transformations/templates/calibrated/louisiana/model_input_variables_louisiana_se_calibrated.xlsx
+++ b/louisiana/transformations/templates/calibrated/louisiana/model_input_variables_louisiana_se_calibrated.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
     <sheet name="strategy_id-6004" sheetId="2" r:id="rId2"/>
+    <sheet name="strategy_id-6006" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="58">
   <si>
     <t>subsector</t>
   </si>
@@ -2321,4 +2322,279 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>0.9782608695652174</v>
+      </c>
+      <c r="X2">
+        <v>0.9565217391304348</v>
+      </c>
+      <c r="Y2">
+        <v>0.9347826086956521</v>
+      </c>
+      <c r="Z2">
+        <v>0.9130434782608696</v>
+      </c>
+      <c r="AA2">
+        <v>0.891304347826087</v>
+      </c>
+      <c r="AB2">
+        <v>0.8695652173913043</v>
+      </c>
+      <c r="AC2">
+        <v>0.8478260869565217</v>
+      </c>
+      <c r="AD2">
+        <v>0.8260869565217391</v>
+      </c>
+      <c r="AE2">
+        <v>0.8043478260869565</v>
+      </c>
+      <c r="AF2">
+        <v>0.7826086956521739</v>
+      </c>
+      <c r="AG2">
+        <v>0.7608695652173914</v>
+      </c>
+      <c r="AH2">
+        <v>0.7391304347826086</v>
+      </c>
+      <c r="AI2">
+        <v>0.7173913043478262</v>
+      </c>
+      <c r="AJ2">
+        <v>0.6956521739130435</v>
+      </c>
+      <c r="AK2">
+        <v>0.6739130434782609</v>
+      </c>
+      <c r="AL2">
+        <v>0.6521739130434783</v>
+      </c>
+      <c r="AM2">
+        <v>0.6304347826086957</v>
+      </c>
+      <c r="AN2">
+        <v>0.6086956521739131</v>
+      </c>
+      <c r="AO2">
+        <v>0.5869565217391304</v>
+      </c>
+      <c r="AP2">
+        <v>0.5652173913043479</v>
+      </c>
+      <c r="AQ2">
+        <v>0.5434782608695652</v>
+      </c>
+      <c r="AR2">
+        <v>0.5217391304347826</v>
+      </c>
+      <c r="AS2">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>